<commit_message>
Rhombus and Draw/fill clr Beta version (waiting for selected function(s))
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COMPUTER\Desktop\Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="11835"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="11832"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,32 +74,56 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="178"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="178"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="178"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +154,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -254,10 +293,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,12 +312,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -295,8 +330,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -304,6 +353,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -352,7 +404,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -385,9 +437,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,6 +489,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -599,56 +685,56 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="14.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="8" width="14.296875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.09765625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -663,22 +749,22 @@
       <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="12"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="7" t="s">
+      <c r="J4" s="6"/>
+      <c r="K4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="9"/>
+      <c r="L4" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -700,7 +786,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -712,7 +798,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new tasks + switch
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COMPUTER\Desktop\Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BCB78B-50AF-4F46-9B76-353D2B86AD2F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Draw Bar</t>
   </si>
@@ -42,9 +36,6 @@
     <t>line</t>
   </si>
   <si>
-    <t>switch &lt;=&gt;</t>
-  </si>
-  <si>
     <t>triangle</t>
   </si>
   <si>
@@ -70,17 +61,44 @@
   </si>
   <si>
     <t>not done</t>
+  </si>
+  <si>
+    <t>Tool Bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch </t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>save (type)</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>copy</t>
+  </si>
+  <si>
+    <t>cut</t>
+  </si>
+  <si>
+    <t>paste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -88,19 +106,19 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,12 +149,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -186,21 +198,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="double">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="1"/>
@@ -229,19 +226,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -262,6 +246,36 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -269,45 +283,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -370,7 +390,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -403,26 +423,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -455,23 +458,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -647,17 +633,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="14.19921875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.09765625" style="1"/>
+    <col min="1" max="8" width="14.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -679,61 +665,98 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="13" t="s">
         <v>6</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="9"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L4" s="4"/>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A4:H4"/>
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
@@ -747,24 +770,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
all tasks done /akram
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="11835"/>
@@ -114,12 +114,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -127,20 +127,20 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -411,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -452,10 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -485,7 +482,16 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -506,7 +512,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="سمة Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -580,6 +586,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -614,6 +621,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -789,70 +797,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.75" style="1" customWidth="1"/>
-    <col min="2" max="9" width="14.375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="1.375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
+    <col min="2" max="9" width="14.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.42578125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="18" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="21" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22"/>
     </row>
-    <row r="2" spans="1:15" ht="33.75" customHeight="1">
+    <row r="2" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:15" ht="29.25" customHeight="1">
+    <row r="3" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="6" t="s">
         <v>8</v>
@@ -879,25 +887,25 @@
         <v>11</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
-    <row r="5" spans="1:15" ht="27">
+    <row r="5" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
       <c r="J5" s="10"/>
       <c r="L5" s="2" t="s">
         <v>13</v>
@@ -908,7 +916,7 @@
       </c>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="6" t="s">
         <v>20</v>
@@ -936,7 +944,7 @@
       </c>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:15" ht="15" thickBot="1">
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -948,53 +956,53 @@
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="1:15" ht="36" customHeight="1" thickTop="1">
+    <row r="8" spans="1:15" ht="36" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:15" ht="27">
+    <row r="9" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="C10" s="25"/>
+      <c r="D10" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16" t="s">
+      <c r="E10" s="27"/>
+      <c r="F10" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="16"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -1008,17 +1016,17 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B5:I5"/>
@@ -1029,24 +1037,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>